<commit_message>
trying as html table
</commit_message>
<xml_diff>
--- a/Source/ADM-OSC_next_v1.xlsx
+++ b/Source/ADM-OSC_next_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\architecture\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.zbyszynski/GIT/ADM-OSC/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9BD1F1D-6756-46FA-8F9E-125C6BD0C0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823CE644-825B-7642-B3FC-F1DE5466726C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3832" yWindow="3188" windowWidth="21601" windowHeight="11534" xr2:uid="{40CF93BD-3817-4C94-A0DF-B537507917E4}"/>
+    <workbookView xWindow="1620" yWindow="2100" windowWidth="25740" windowHeight="14300" xr2:uid="{40CF93BD-3817-4C94-A0DF-B537507917E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Next version (+Dolby)" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="180">
   <si>
     <t>Dynamic/real-time</t>
   </si>
@@ -567,6 +567,15 @@
   </si>
   <si>
     <t>/dprog</t>
+  </si>
+  <si>
+    <t>/refdistance</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t>normalized</t>
   </si>
 </sst>
 </file>
@@ -837,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -961,12 +970,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1302,23 +1305,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB00DDCA-C3FE-C747-B425-7819D265B928}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="99" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.5625" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="7" max="7" width="13.0625" customWidth="1"/>
-    <col min="12" max="12" width="15.5625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.3125" style="40" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" style="40" customWidth="1"/>
     <col min="17" max="17" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="37" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:20" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -1341,20 +1344,20 @@
       <c r="S1" s="41"/>
       <c r="T1" s="41"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A2" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="50" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
@@ -1370,12 +1373,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
       <c r="F3" t="s">
         <v>12</v>
       </c>
@@ -1389,12 +1392,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -1408,12 +1411,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
       <c r="F5" t="s">
         <v>16</v>
       </c>
@@ -1427,12 +1430,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
       <c r="F6" t="s">
         <v>20</v>
       </c>
@@ -1443,12 +1446,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="13.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+    <row r="7" spans="1:20" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
       <c r="F7" t="s">
         <v>22</v>
       </c>
@@ -1459,12 +1462,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="F8" t="s">
         <v>24</v>
       </c>
@@ -1475,12 +1478,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" t="s">
         <v>26</v>
       </c>
@@ -1491,12 +1494,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" t="s">
         <v>28</v>
       </c>
@@ -1510,20 +1513,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52" t="s">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="50" t="s">
         <v>6</v>
       </c>
       <c r="H11" t="s">
@@ -1536,14 +1539,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" t="s">
         <v>12</v>
       </c>
@@ -1551,14 +1554,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
       <c r="H13" t="s">
         <v>14</v>
       </c>
@@ -1566,14 +1569,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
       <c r="H14" t="s">
         <v>16</v>
       </c>
@@ -1581,14 +1584,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
+    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
       <c r="H15" t="s">
         <v>20</v>
       </c>
@@ -1596,14 +1599,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
       <c r="H16" t="s">
         <v>22</v>
       </c>
@@ -1611,14 +1614,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
       <c r="H17" t="s">
         <v>24</v>
       </c>
@@ -1626,14 +1629,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -1641,14 +1644,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
       <c r="H19" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="37" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:20" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>34</v>
       </c>
@@ -1671,17 +1674,17 @@
       <c r="S20" s="41"/>
       <c r="T20" s="41"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="53" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A21" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="51" t="s">
         <v>35</v>
       </c>
       <c r="E21" t="s">
@@ -1697,12 +1700,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54" t="s">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52" t="s">
         <v>70</v>
       </c>
       <c r="F22" t="s">
@@ -1712,12 +1715,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A23" s="51"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
       <c r="F23" t="s">
         <v>73</v>
       </c>
@@ -1725,12 +1728,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
       <c r="F24" t="s">
         <v>75</v>
       </c>
@@ -1738,39 +1741,39 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="50" t="s">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A25" s="51"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="38" t="s">
         <v>175</v>
       </c>
       <c r="K25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="50" t="s">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="38" t="s">
         <v>176</v>
       </c>
       <c r="K26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53" t="s">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="53" t="s">
+      <c r="F27" s="51" t="s">
         <v>6</v>
       </c>
       <c r="G27" t="s">
@@ -1779,621 +1782,644 @@
       <c r="K27" t="s">
         <v>10</v>
       </c>
+      <c r="L27" t="s">
+        <v>178</v>
+      </c>
       <c r="N27" s="48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
+    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="51"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
       <c r="G28" t="s">
+        <v>177</v>
+      </c>
+      <c r="K28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" t="s">
+        <v>179</v>
+      </c>
+      <c r="N28" s="48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" t="s">
         <v>42</v>
-      </c>
-      <c r="K28" t="s">
-        <v>43</v>
-      </c>
-      <c r="P28" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q28" s="47"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A29" s="53"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" t="s">
-        <v>45</v>
       </c>
       <c r="K29" t="s">
         <v>43</v>
       </c>
-      <c r="P29" s="42" t="s">
+      <c r="P29" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q29" s="47"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A30" s="51"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P30" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="Q29" s="43" t="s">
+      <c r="Q30" s="43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A30" s="53"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" t="s">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" t="s">
         <v>48</v>
-      </c>
-      <c r="K30" t="s">
-        <v>49</v>
-      </c>
-      <c r="P30" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q30" s="43" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A31" s="53"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" t="s">
-        <v>52</v>
       </c>
       <c r="K31" t="s">
         <v>49</v>
       </c>
-      <c r="N31" s="48" t="s">
-        <v>53</v>
-      </c>
       <c r="P31" s="42" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q31" s="43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A32" s="53"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A32" s="51"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
       <c r="G32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K32" t="s">
         <v>49</v>
       </c>
+      <c r="N32" s="48" t="s">
+        <v>53</v>
+      </c>
       <c r="P32" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q32" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A33" s="51"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" t="s">
+        <v>49</v>
+      </c>
+      <c r="P33" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="Q32" s="43" t="s">
+      <c r="Q33" s="43" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" t="s">
+    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="51"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" t="s">
         <v>59</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K34" t="s">
         <v>10</v>
       </c>
-      <c r="P33" s="44" t="s">
+      <c r="P34" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="Q33" s="45" t="s">
+      <c r="Q34" s="45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="54" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A35" s="51"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>63</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
-      <c r="H35" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A36" s="51"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="52"/>
+      <c r="H36" t="s">
         <v>64</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A36" s="53"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="54"/>
-      <c r="H36" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" t="s">
         <v>174</v>
-      </c>
-      <c r="K36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="16.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="53"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" t="s">
-        <v>45</v>
       </c>
       <c r="K37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="53"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
+    <row r="38" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="51"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>6</v>
+      </c>
       <c r="G38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A39" s="51"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" t="s">
         <v>48</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="53"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" t="s">
+    <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="51"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" t="s">
         <v>66</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K40" t="s">
         <v>43</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>67</v>
       </c>
-      <c r="M39" s="40" t="s">
+      <c r="M40" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="N39" s="48" t="s">
+      <c r="N40" s="48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A41" s="51"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="53" t="s">
+      <c r="E41" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="53" t="s">
+      <c r="F41" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="53" t="s">
+      <c r="G41" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H41" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I41" t="s">
         <v>52</v>
-      </c>
-      <c r="K40" t="s">
-        <v>49</v>
-      </c>
-      <c r="P40" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q40" s="47" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="53"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" t="s">
-        <v>48</v>
       </c>
       <c r="K41" t="s">
         <v>49</v>
       </c>
-      <c r="P41" s="42" t="s">
+      <c r="P41" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q41" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A42" s="51"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" t="s">
+        <v>49</v>
+      </c>
+      <c r="P42" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="Q41" s="43">
+      <c r="Q42" s="43">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53" t="s">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A43" s="51"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="H42" s="53" t="s">
+      <c r="H43" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>45</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K43" t="s">
         <v>43</v>
       </c>
-      <c r="P42" s="42" t="s">
+      <c r="P43" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="Q42" s="43">
+      <c r="Q43" s="43">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A43" s="53"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" t="s">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A44" s="51"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" t="s">
         <v>48</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K44" t="s">
         <v>49</v>
       </c>
-      <c r="N43" s="48" t="s">
+      <c r="N44" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="P43" s="42" t="s">
+      <c r="P44" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="Q43" s="43">
+      <c r="Q44" s="43">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" t="s">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A45" s="51"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" t="s">
         <v>66</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K45" t="s">
         <v>43</v>
       </c>
-      <c r="P44" s="42" t="s">
+      <c r="P45" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="Q44" s="43">
+      <c r="Q45" s="43">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A46" s="51"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" t="s">
         <v>59</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K46" t="s">
         <v>10</v>
       </c>
-      <c r="P45" s="42" t="s">
+      <c r="P46" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="Q45" s="43">
+      <c r="Q46" s="43">
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" s="53"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A47" s="51"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="H46" s="53" t="s">
+      <c r="H47" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="51" t="s">
+      <c r="K47" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="P46" s="42" t="s">
+      <c r="P47" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="Q46" s="43">
+      <c r="Q47" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="13.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" t="s">
+    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="51"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" t="s">
         <v>42</v>
-      </c>
-      <c r="K47" t="s">
-        <v>43</v>
-      </c>
-      <c r="P47" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q47" s="45">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="53"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" t="s">
-        <v>45</v>
       </c>
       <c r="K48" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A49" s="53"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
+      <c r="P48" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q48" s="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A49" s="51"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
       <c r="I49" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A50" s="51"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" t="s">
         <v>48</v>
-      </c>
-      <c r="K49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" t="s">
-        <v>52</v>
       </c>
       <c r="K50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="53"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
       <c r="I51" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="53"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A52" s="51"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" t="s">
+        <v>56</v>
+      </c>
+      <c r="K52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A53" s="51"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="51"/>
+      <c r="I53" t="s">
         <v>59</v>
       </c>
-      <c r="K52" t="s">
+      <c r="K53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="53"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="51" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A54" s="51"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J54" t="s">
         <v>63</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="53"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="51"/>
-      <c r="J54" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A55" s="51"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="49"/>
+      <c r="J55" t="s">
         <v>64</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K55" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="53"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="53"/>
-      <c r="I55" s="51"/>
-      <c r="J55" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A56" s="51"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="49"/>
+      <c r="J56" t="s">
         <v>174</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="53"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="50" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A57" s="51"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="38" t="s">
         <v>48</v>
-      </c>
-      <c r="K56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" t="s">
-        <v>52</v>
       </c>
       <c r="K57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A58" s="49"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A58" s="51"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
+      <c r="G58" t="s">
+        <v>52</v>
+      </c>
+      <c r="K58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A59" s="49"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="28">
-    <mergeCell ref="F40:F57"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="E27:E36"/>
-    <mergeCell ref="F27:F36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="G46:G55"/>
-    <mergeCell ref="H46:H55"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A21:A57"/>
-    <mergeCell ref="B21:B57"/>
-    <mergeCell ref="C21:C57"/>
-    <mergeCell ref="D40:D57"/>
-    <mergeCell ref="E40:E57"/>
+    <mergeCell ref="F41:F58"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="E27:E37"/>
+    <mergeCell ref="F27:F37"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G47:G56"/>
+    <mergeCell ref="H47:H56"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="A21:A58"/>
+    <mergeCell ref="B21:B58"/>
+    <mergeCell ref="C21:C58"/>
+    <mergeCell ref="D41:D58"/>
+    <mergeCell ref="E41:E58"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="D21:D39"/>
+    <mergeCell ref="D21:D40"/>
     <mergeCell ref="F11:F19"/>
     <mergeCell ref="G11:G19"/>
     <mergeCell ref="A2:A19"/>
@@ -2420,34 +2446,34 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.8125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.0625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="5.5625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.5625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="7.3125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.3125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.0625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25" style="2" customWidth="1"/>
     <col min="11" max="11" width="11" style="2" customWidth="1"/>
-    <col min="12" max="12" width="35.0625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="35" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>85</v>
       </c>
@@ -2485,7 +2511,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>97</v>
       </c>
@@ -2523,7 +2549,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>97</v>
       </c>
@@ -2559,7 +2585,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>97</v>
       </c>
@@ -2597,7 +2623,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>97</v>
       </c>
@@ -2610,12 +2636,12 @@
       <c r="D8" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="57"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
       <c r="I8" s="10" t="s">
         <v>117</v>
       </c>
@@ -2629,7 +2655,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>119</v>
       </c>
@@ -2667,7 +2693,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>124</v>
       </c>
@@ -2697,7 +2723,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>126</v>
       </c>
@@ -2727,12 +2753,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -2770,7 +2796,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>97</v>
       </c>
@@ -2808,7 +2834,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
@@ -2846,7 +2872,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>97</v>
       </c>
@@ -2884,7 +2910,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>97</v>
       </c>
@@ -2897,12 +2923,12 @@
       <c r="D18" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="57"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="55"/>
       <c r="I18" s="26" t="s">
         <v>145</v>
       </c>
@@ -2916,7 +2942,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>119</v>
       </c>
@@ -2946,7 +2972,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>126</v>
       </c>
@@ -2976,7 +3002,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>124</v>
       </c>
@@ -3006,12 +3032,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>85</v>
       </c>
@@ -3047,7 +3073,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="81" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.15">
       <c r="A25" s="11" t="s">
         <v>151</v>
       </c>
@@ -3083,18 +3109,18 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="L26" s="13"/>
     </row>
-    <row r="27" spans="1:12" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>157</v>
       </c>
       <c r="L27" s="13"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>85</v>
       </c>
@@ -3130,7 +3156,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
         <v>158</v>
       </c>
@@ -3166,27 +3192,27 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" s="20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>85</v>
       </c>
@@ -3222,7 +3248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.15">
       <c r="A37" s="11" t="s">
         <v>168</v>
       </c>
@@ -3274,6 +3300,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="bcbf2e4c-81be-4766-b8fe-543c567d4382">In progress</Status>
+    <TaxCatchAll xmlns="b7f74b8f-5815-417a-ba55-57e4d39845e1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bcbf2e4c-81be-4766-b8fe-543c567d4382">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD31288C2C9D7D4DABF7DD8413342462" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b4582ae8613078b24fcbd390247d8dc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcbf2e4c-81be-4766-b8fe-543c567d4382" xmlns:ns3="e751ee4b-bd23-453e-97e1-76efacbc5558" xmlns:ns4="b7f74b8f-5815-417a-ba55-57e4d39845e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd6f936881d299348c3084c4aea058f3" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bcbf2e4c-81be-4766-b8fe-543c567d4382"/>
@@ -3531,28 +3578,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="bcbf2e4c-81be-4766-b8fe-543c567d4382">In progress</Status>
-    <TaxCatchAll xmlns="b7f74b8f-5815-417a-ba55-57e4d39845e1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bcbf2e4c-81be-4766-b8fe-543c567d4382">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8051EBB2-9E71-4327-BC0C-06CBA46F82CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bcbf2e4c-81be-4766-b8fe-543c567d4382"/>
+    <ds:schemaRef ds:uri="b7f74b8f-5815-417a-ba55-57e4d39845e1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8002FD75-981C-4A93-8DA7-E1B761E86C87}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A3E8DD0-14D7-4481-8446-3F6B37F8DD3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3570,23 +3615,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8051EBB2-9E71-4327-BC0C-06CBA46F82CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bcbf2e4c-81be-4766-b8fe-543c567d4382"/>
-    <ds:schemaRef ds:uri="b7f74b8f-5815-417a-ba55-57e4d39845e1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8002FD75-981C-4A93-8DA7-E1B761E86C87}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>